<commit_message>
added test cases for streaming sever
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/ad_blocking_server/ad_blocking_server.xlsx
+++ b/apps/features/backlog/desktop/windows/ad_blocking_server/ad_blocking_server.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\ad_blocking_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91601A2-62A3-4262-89CB-EB197539C782}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A801C3-A7C1-4D6D-97F7-3330177BAB7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="ad_blocking_server" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,16 +95,6 @@
     <t>TC_SYM_ABS_006</t>
   </si>
   <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. Enter your password in the password field.
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the third ad-blocking server from the ad-blocking section.
-7. Visit  bangla.bdnew24.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
     <t>Try to See Ads the Server No.3 for Ads Blocking Server with bangla.bdnew24.com news website</t>
   </si>
   <si>
@@ -115,16 +105,6 @@
   </si>
   <si>
     <t>Try to See Ads the Server No.3 for Ads Blocking Server with prothomalo.com news website</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. Enter your password in the password field.
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the third ad-blocking server from the ad-blocking section.
-7. Visit  cricinfo.com
-8. Start browsing the website.</t>
   </si>
   <si>
     <t>Try to See Ads the Server No.3 for Ads Blocking Server with cricinfo.com news website</t>
@@ -139,76 +119,6 @@
     <t>Test Scenario: add blocking server in home page</t>
   </si>
   <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the first ad-blocking server from the ad-blocking section.
-7. Visit  bangla.bdnew24.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page..
-6. Select the first ad-blocking server from the ad-blocking section.
-7. Visit  prothomalo.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the first ad-blocking server from the ad-blocking section.
-7. Visit  cricinfo.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the second ad-blocking server from the ad-blocking section.
-7. Visit  bangla.bdnew24.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page..
-6. Select the second ad-blocking server from the ad-blocking section.
-7. Visit  prothomalo.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the second ad-blocking server from the ad-blocking section.
-7. Visit  cricinfo.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
-    <t>1. Go to the Google Play Store and install SymlexVPN on your mobile device.
-2. Open the SymlexVPN application once it's installed.
-3. login with credentials
-4. Tap the login button
-5. Navigate to the server list page.
-6. Select the third ad-blocking server from the ad-blocking section.
-7. Visit  bangla.bdnew24.com
-8. Start browsing the website.</t>
-  </si>
-  <si>
     <t>TC_SYM_ABS_010</t>
   </si>
   <si>
@@ -218,26 +128,10 @@
     <t>should be well visible</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check the visibility of ad blocking servers</t>
-  </si>
-  <si>
     <t>check the dynamic ad blocking</t>
   </si>
   <si>
     <t>TC_SYM_ABS_011</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check the dynamic ad blocking</t>
   </si>
   <si>
     <t>ad-blocking servers should handle different ad 
@@ -245,14 +139,6 @@
   </si>
   <si>
     <t>check ad blocking consistency</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to connect to multiple servers from the "ad blocking server" list</t>
   </si>
   <si>
     <t>ad blocking should be consistently applied across 
@@ -263,14 +149,6 @@
   </si>
   <si>
     <t>check the impact on page load time</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to measure the impact of ad blocking on the overall page load time</t>
   </si>
   <si>
     <t>ad-blocking servers should provide a reasonable 
@@ -286,14 +164,6 @@
     <t>TC_SYM_ABS_014</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check if the user interface provides information about the ad-blocking status when connected to an "ad blocking server."</t>
-  </si>
-  <si>
     <t>should confirm that users can easily identify 
 whether the ad-blocking feature is active</t>
   </si>
@@ -302,14 +172,6 @@
   </si>
   <si>
     <t>TC_SYM_ABS_015</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check if the application allows users to customize ad-blocking settings (e.g., whitelist certain domains)</t>
   </si>
   <si>
     <t>should confirm that users have some control over
@@ -322,23 +184,7 @@
     <t>TC_SYM_ABS_016</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test the ad-blocking servers with different web browsers (e.g., Chrome, Firefox)</t>
-  </si>
-  <si>
     <t>check ad blocking on mobile devices</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to check ad blocking on mobile devices</t>
   </si>
   <si>
     <t>TC_SYM_ABS_017</t>
@@ -354,14 +200,6 @@
     <t>check user feedback for ad blocking</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to Connect to an "ad blocking server" and visit websites known for displaying ads</t>
-  </si>
-  <si>
     <t>should verify that the application provides positive
  feedback indicating successful ad blocking</t>
   </si>
@@ -370,14 +208,6 @@
   </si>
   <si>
     <t>TC_SYM_ABS_019</t>
-  </si>
-  <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test ad-blocking with various ad formats, including banners, pop-ups, and video ads</t>
   </si>
   <si>
     <t>should confirm that the ad-blocking servers 
@@ -390,14 +220,6 @@
     <t>check ad blocking with secure connections</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to test the ad-blocking servers with websites using https</t>
-  </si>
-  <si>
     <t>should confirm that ad blocking works seamlessly 
 with secure (encrypted) connections</t>
   </si>
@@ -408,20 +230,198 @@
     <t>TC_SYM_ABS_021</t>
   </si>
   <si>
-    <t>1. go to the google play store and install symlexvpn on your mobile device.
-2. open the symlexvpn application once it's installed.
-3. login with credentials
-4. tap the login button
-5. navigate to the server list page..
-6. try to simulate a high number of users connecting to ad-blocking servers simultaneously</t>
-  </si>
-  <si>
     <t>verify that the servers maintain their ad-blocking 
 functionality under increased load</t>
   </si>
   <si>
     <t>should confirm that the ad-blocking functionality 
 is consistent across various browsers</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. Enter your password in the password field.
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the third ad-blocking server from the ad-blocking section.
+7. Visit  cricinfo.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check the visibility of ad blocking servers</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the first ad-blocking server from the ad-blocking section.
+7. Visit  bangla.bdnew24.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page..
+6. Select the first ad-blocking server from the ad-blocking section.
+7. Visit  prothomalo.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the first ad-blocking server from the ad-blocking section.
+7. Visit  cricinfo.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the second ad-blocking server from the ad-blocking section.
+7. Visit  bangla.bdnew24.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page..
+6. Select the second ad-blocking server from the ad-blocking section.
+7. Visit  prothomalo.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the second ad-blocking server from the ad-blocking section.
+7. Visit  cricinfo.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. login with credentials
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the third ad-blocking server from the ad-blocking section.
+7. Visit  bangla.bdnew24.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. Open the SymlexVPN application once it's installed.
+3. Enter your password in the password field.
+4. Tap the login button
+5. Navigate to the server list page.
+6. Select the third ad-blocking server from the ad-blocking section.
+7. Visit  bangla.bdnew24.com
+8. Start browsing the website.</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check the dynamic ad blocking</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to connect to multiple servers from the "ad blocking server" list</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to measure the impact of ad blocking on the overall page load time</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check if the user interface provides information about the ad-blocking status when connected to an "ad blocking server."</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check if the application allows users to customize ad-blocking settings (e.g., whitelist certain domains)</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test the ad-blocking servers with different web browsers (e.g., Chrome, Firefox)</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to check ad blocking on mobile devices</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to Connect to an "ad blocking server" and visit websites known for displaying ads</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test ad-blocking with various ad formats, including banners, pop-ups, and video ads</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to test the ad-blocking servers with websites using https</t>
+  </si>
+  <si>
+    <t>1. go to the google app store and install symlexvpn on your desktop device
+2. open the symlexvpn application once it's installed.
+3. login with credentials
+4. tap the login button
+5. navigate to the server list page..
+6. try to simulate a high number of users connecting to ad-blocking servers simultaneously</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1527,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1546,7 +1546,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1649,13 +1649,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
@@ -1691,13 +1691,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>10</v>
@@ -1733,13 +1733,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>10</v>
@@ -1773,13 +1773,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>10</v>
@@ -1813,13 +1813,13 @@
         <v>20</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>10</v>
@@ -1853,13 +1853,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>10</v>
@@ -1890,16 +1890,16 @@
     </row>
     <row r="10" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>10</v>
@@ -1930,16 +1930,16 @@
     </row>
     <row r="11" spans="1:26" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>10</v>
@@ -1970,16 +1970,16 @@
     </row>
     <row r="12" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>10</v>
@@ -2010,19 +2010,19 @@
     </row>
     <row r="13" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="18"/>
@@ -2048,19 +2048,19 @@
     </row>
     <row r="14" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -2086,19 +2086,19 @@
     </row>
     <row r="15" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -2124,19 +2124,19 @@
     </row>
     <row r="16" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -2162,19 +2162,19 @@
     </row>
     <row r="17" spans="1:26" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="18" spans="1:26" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -2238,19 +2238,19 @@
     </row>
     <row r="19" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -2276,19 +2276,19 @@
     </row>
     <row r="20" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -2314,19 +2314,19 @@
     </row>
     <row r="21" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -2352,19 +2352,19 @@
     </row>
     <row r="22" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
@@ -2390,19 +2390,19 @@
     </row>
     <row r="23" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
@@ -2428,19 +2428,19 @@
     </row>
     <row r="24" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>

</xml_diff>